<commit_message>
Update IP - EX 15 - Gerenciador de nomes (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 15 - Gerenciador de nomes (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 15 - Gerenciador de nomes (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73641786-3F5F-402D-8818-56B7637987C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC456B6-CB65-401A-89DF-024FF177F915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="4" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <definedName name="Mar">EXPLICAÇÃO!$F$10:$F$14</definedName>
     <definedName name="Marcos">EXPLICAÇÃO!$D$14:$G$14</definedName>
     <definedName name="Matheus">EXPLICAÇÃO!$D$10:$G$10</definedName>
+    <definedName name="Valor_dolar">EXERCICIOS!$K$10</definedName>
     <definedName name="Valor_final_Exportação">EXERCICIOS!$F$10:$F$87</definedName>
     <definedName name="Vendas_un">EXERCICIOS!$E$10:$E$87</definedName>
     <definedName name="Vendas_valor">EXERCICIOS!$D$10:$D$87</definedName>
@@ -451,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -536,15 +537,8 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -773,7 +767,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>485375</xdr:colOff>
+      <xdr:colOff>380600</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>85693</xdr:rowOff>
     </xdr:to>
@@ -1222,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2F6FA6-A305-4CB2-A573-C40DFFE7E434}">
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1233,96 +1227,96 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="48"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="48"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="51"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="51"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="54"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
     </row>
     <row r="7" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
@@ -1430,7 +1424,7 @@
   <dimension ref="B1:Q19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,103 +1432,102 @@
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="29" customWidth="1"/>
-    <col min="6" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="48"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="48"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="51"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="51"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="54"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
     </row>
     <row r="8" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -1646,25 +1639,49 @@
       <c r="H14" s="32"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
+      <c r="D15" s="41">
+        <f>SUM(Jan)</f>
+        <v>1680</v>
+      </c>
+      <c r="E15" s="41">
+        <f>SUM(Fev)</f>
+        <v>1891</v>
+      </c>
+      <c r="F15" s="41">
+        <f>SUM(Mar)</f>
+        <v>1377</v>
+      </c>
+      <c r="G15" s="41">
+        <f>SUM(Abr)</f>
+        <v>1338</v>
+      </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
+      <c r="D16" s="39">
+        <f>MEDIAN(Jan)</f>
+        <v>302</v>
+      </c>
+      <c r="E16" s="39">
+        <f>MEDIAN(Fev)</f>
+        <v>406</v>
+      </c>
+      <c r="F16" s="39">
+        <f>MEDIAN(Mar)</f>
+        <v>220</v>
+      </c>
+      <c r="G16" s="39">
+        <f>MEDIAN(Abr)</f>
+        <v>287</v>
+      </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="42" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1682,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:Q88"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1699,96 +1716,96 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="48"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="48"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="51"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="51"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="54"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="51"/>
     </row>
     <row r="7" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G7" s="1"/>
@@ -1820,7 +1837,10 @@
       <c r="E10" s="28">
         <v>10</v>
       </c>
-      <c r="F10" s="26"/>
+      <c r="F10" s="26">
+        <f>PRODUCT(D10,Valor_dolar)</f>
+        <v>2621.4299999999998</v>
+      </c>
       <c r="J10" s="20" t="s">
         <v>20</v>
       </c>
@@ -1838,7 +1858,10 @@
       <c r="E11" s="28">
         <v>7</v>
       </c>
-      <c r="F11" s="26"/>
+      <c r="F11" s="26">
+        <f>PRODUCT(D11,Valor_dolar)</f>
+        <v>4216.8599999999997</v>
+      </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C12" s="24" t="s">
@@ -1850,11 +1873,17 @@
       <c r="E12" s="28">
         <v>7</v>
       </c>
-      <c r="F12" s="26"/>
+      <c r="F12" s="26">
+        <f>PRODUCT(D12,Valor_dolar)</f>
+        <v>3514.0499999999997</v>
+      </c>
       <c r="J12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="19"/>
+      <c r="K12" s="19">
+        <f>SUM(Valor_final_Exportação)</f>
+        <v>295159.68000000011</v>
+      </c>
     </row>
     <row r="13" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="24" t="s">
@@ -1866,7 +1895,10 @@
       <c r="E13" s="28">
         <v>2</v>
       </c>
-      <c r="F13" s="26"/>
+      <c r="F13" s="26">
+        <f>PRODUCT(D13,Valor_dolar)</f>
+        <v>3170.34</v>
+      </c>
       <c r="J13" s="21"/>
       <c r="K13" s="17"/>
     </row>
@@ -1880,11 +1912,17 @@
       <c r="E14" s="28">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="26">
+        <f>PRODUCT(D14,Valor_dolar)</f>
+        <v>2606.04</v>
+      </c>
       <c r="J14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="18"/>
+      <c r="K14" s="18">
+        <f ca="1">SUM(Vendas_un)</f>
+        <v>662</v>
+      </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C15" s="24" t="s">
@@ -1896,7 +1934,10 @@
       <c r="E15" s="28">
         <v>7</v>
       </c>
-      <c r="F15" s="26"/>
+      <c r="F15" s="26">
+        <f>PRODUCT(D15,Valor_dolar)</f>
+        <v>3211.38</v>
+      </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="24" t="s">
@@ -1908,7 +1949,10 @@
       <c r="E16" s="28">
         <v>9</v>
       </c>
-      <c r="F16" s="26"/>
+      <c r="F16" s="26">
+        <f>PRODUCT(D16,Valor_dolar)</f>
+        <v>3088.2599999999998</v>
+      </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="24" t="s">
@@ -1920,7 +1964,10 @@
       <c r="E17" s="28">
         <v>5</v>
       </c>
-      <c r="F17" s="26"/>
+      <c r="F17" s="26">
+        <f>PRODUCT(D17,Valor_dolar)</f>
+        <v>3431.97</v>
+      </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="24" t="s">
@@ -1932,7 +1979,10 @@
       <c r="E18" s="28">
         <v>6</v>
       </c>
-      <c r="F18" s="26"/>
+      <c r="F18" s="26">
+        <f>PRODUCT(D18,Valor_dolar)</f>
+        <v>4309.2</v>
+      </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="24" t="s">
@@ -1944,7 +1994,10 @@
       <c r="E19" s="28">
         <v>9</v>
       </c>
-      <c r="F19" s="26"/>
+      <c r="F19" s="26">
+        <f>PRODUCT(D19,Valor_dolar)</f>
+        <v>3632.04</v>
+      </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="24" t="s">
@@ -1956,7 +2009,10 @@
       <c r="E20" s="28">
         <v>3</v>
       </c>
-      <c r="F20" s="26"/>
+      <c r="F20" s="26">
+        <f>PRODUCT(D20,Valor_dolar)</f>
+        <v>2765.07</v>
+      </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="24" t="s">
@@ -1968,7 +2024,10 @@
       <c r="E21" s="28">
         <v>10</v>
       </c>
-      <c r="F21" s="26"/>
+      <c r="F21" s="26">
+        <f>PRODUCT(D21,Valor_dolar)</f>
+        <v>4714.47</v>
+      </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="24" t="s">
@@ -1980,7 +2039,10 @@
       <c r="E22" s="28">
         <v>5</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="26">
+        <f>PRODUCT(D22,Valor_dolar)</f>
+        <v>4888.8900000000003</v>
+      </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="24" t="s">
@@ -1992,7 +2054,10 @@
       <c r="E23" s="28">
         <v>6</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="26">
+        <f>PRODUCT(D23,Valor_dolar)</f>
+        <v>4540.05</v>
+      </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="24" t="s">
@@ -2004,7 +2069,10 @@
       <c r="E24" s="28">
         <v>4</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="26">
+        <f>PRODUCT(D24,Valor_dolar)</f>
+        <v>3355.02</v>
+      </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="24" t="s">
@@ -2016,7 +2084,10 @@
       <c r="E25" s="28">
         <v>2</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="26">
+        <f>PRODUCT(D25,Valor_dolar)</f>
+        <v>4411.8</v>
+      </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="24" t="s">
@@ -2028,7 +2099,10 @@
       <c r="E26" s="28">
         <v>8</v>
       </c>
-      <c r="F26" s="26"/>
+      <c r="F26" s="26">
+        <f>PRODUCT(D26,Valor_dolar)</f>
+        <v>4724.7299999999996</v>
+      </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="24" t="s">
@@ -2040,7 +2114,10 @@
       <c r="E27" s="28">
         <v>10</v>
       </c>
-      <c r="F27" s="26"/>
+      <c r="F27" s="26">
+        <f>PRODUCT(D27,Valor_dolar)</f>
+        <v>3939.84</v>
+      </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="24" t="s">
@@ -2052,7 +2129,10 @@
       <c r="E28" s="28">
         <v>4</v>
       </c>
-      <c r="F28" s="26"/>
+      <c r="F28" s="26">
+        <f>PRODUCT(D28,Valor_dolar)</f>
+        <v>3113.91</v>
+      </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="24" t="s">
@@ -2064,7 +2144,10 @@
       <c r="E29" s="28">
         <v>7</v>
       </c>
-      <c r="F29" s="26"/>
+      <c r="F29" s="26">
+        <f>PRODUCT(D29,Valor_dolar)</f>
+        <v>2831.7599999999998</v>
+      </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" s="24" t="s">
@@ -2076,7 +2159,10 @@
       <c r="E30" s="28">
         <v>7</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="26">
+        <f>PRODUCT(D30,Valor_dolar)</f>
+        <v>4078.35</v>
+      </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="24" t="s">
@@ -2088,7 +2174,10 @@
       <c r="E31" s="28">
         <v>4</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="26">
+        <f>PRODUCT(D31,Valor_dolar)</f>
+        <v>2565</v>
+      </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="24" t="s">
@@ -2100,7 +2189,10 @@
       <c r="E32" s="28">
         <v>1</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="26">
+        <f>PRODUCT(D32,Valor_dolar)</f>
+        <v>2970.27</v>
+      </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="24" t="s">
@@ -2112,7 +2204,10 @@
       <c r="E33" s="28">
         <v>10</v>
       </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="26">
+        <f>PRODUCT(D33,Valor_dolar)</f>
+        <v>2836.89</v>
+      </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="24" t="s">
@@ -2124,7 +2219,10 @@
       <c r="E34" s="28">
         <v>7</v>
       </c>
-      <c r="F34" s="26"/>
+      <c r="F34" s="26">
+        <f>PRODUCT(D34,Valor_dolar)</f>
+        <v>4617</v>
+      </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="24" t="s">
@@ -2136,7 +2234,10 @@
       <c r="E35" s="28">
         <v>10</v>
       </c>
-      <c r="F35" s="26"/>
+      <c r="F35" s="26">
+        <f>PRODUCT(D35,Valor_dolar)</f>
+        <v>4622.13</v>
+      </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C36" s="24" t="s">
@@ -2148,7 +2249,10 @@
       <c r="E36" s="28">
         <v>6</v>
       </c>
-      <c r="F36" s="26"/>
+      <c r="F36" s="26">
+        <f>PRODUCT(D36,Valor_dolar)</f>
+        <v>3898.7999999999997</v>
+      </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="24" t="s">
@@ -2160,7 +2264,10 @@
       <c r="E37" s="28">
         <v>10</v>
       </c>
-      <c r="F37" s="26"/>
+      <c r="F37" s="26">
+        <f>PRODUCT(D37,Valor_dolar)</f>
+        <v>4411.8</v>
+      </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="24" t="s">
@@ -2172,7 +2279,10 @@
       <c r="E38" s="28">
         <v>4</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="26">
+        <f>PRODUCT(D38,Valor_dolar)</f>
+        <v>4668.3</v>
+      </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C39" s="24" t="s">
@@ -2184,7 +2294,10 @@
       <c r="E39" s="28">
         <v>9</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="26">
+        <f>PRODUCT(D39,Valor_dolar)</f>
+        <v>4524.66</v>
+      </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="24" t="s">
@@ -2196,7 +2309,10 @@
       <c r="E40" s="28">
         <v>10</v>
       </c>
-      <c r="F40" s="26"/>
+      <c r="F40" s="26">
+        <f>PRODUCT(D40,Valor_dolar)</f>
+        <v>4801.68</v>
+      </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" s="24" t="s">
@@ -2208,7 +2324,10 @@
       <c r="E41" s="28">
         <v>9</v>
       </c>
-      <c r="F41" s="26"/>
+      <c r="F41" s="26">
+        <f>PRODUCT(D41,Valor_dolar)</f>
+        <v>3252.42</v>
+      </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" s="24" t="s">
@@ -2220,7 +2339,10 @@
       <c r="E42" s="28">
         <v>10</v>
       </c>
-      <c r="F42" s="26"/>
+      <c r="F42" s="26">
+        <f>PRODUCT(D42,Valor_dolar)</f>
+        <v>2688.12</v>
+      </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C43" s="24" t="s">
@@ -2232,7 +2354,10 @@
       <c r="E43" s="28">
         <v>6</v>
       </c>
-      <c r="F43" s="26"/>
+      <c r="F43" s="26">
+        <f>PRODUCT(D43,Valor_dolar)</f>
+        <v>3355.02</v>
+      </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" s="24" t="s">
@@ -2244,7 +2369,10 @@
       <c r="E44" s="28">
         <v>1</v>
       </c>
-      <c r="F44" s="26"/>
+      <c r="F44" s="26">
+        <f>PRODUCT(D44,Valor_dolar)</f>
+        <v>5017.1400000000003</v>
+      </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" s="24" t="s">
@@ -2256,7 +2384,10 @@
       <c r="E45" s="28">
         <v>4</v>
       </c>
-      <c r="F45" s="26"/>
+      <c r="F45" s="26">
+        <f>PRODUCT(D45,Valor_dolar)</f>
+        <v>4827.33</v>
+      </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" s="24" t="s">
@@ -2268,7 +2399,10 @@
       <c r="E46" s="28">
         <v>8</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="26">
+        <f>PRODUCT(D46,Valor_dolar)</f>
+        <v>2595.7799999999997</v>
+      </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" s="24" t="s">
@@ -2280,7 +2414,10 @@
       <c r="E47" s="28">
         <v>5</v>
       </c>
-      <c r="F47" s="26"/>
+      <c r="F47" s="26">
+        <f>PRODUCT(D47,Valor_dolar)</f>
+        <v>2867.67</v>
+      </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" s="24" t="s">
@@ -2292,7 +2429,10 @@
       <c r="E48" s="28">
         <v>1</v>
       </c>
-      <c r="F48" s="26"/>
+      <c r="F48" s="26">
+        <f>PRODUCT(D48,Valor_dolar)</f>
+        <v>4304.07</v>
+      </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="24" t="s">
@@ -2305,7 +2445,10 @@
         <f ca="1">RANDBETWEEN(1,20)</f>
         <v>2</v>
       </c>
-      <c r="F49" s="26"/>
+      <c r="F49" s="26">
+        <f>PRODUCT(D49,Valor_dolar)</f>
+        <v>2806.11</v>
+      </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="24" t="s">
@@ -2317,7 +2460,10 @@
       <c r="E50" s="30">
         <v>1</v>
       </c>
-      <c r="F50" s="26"/>
+      <c r="F50" s="26">
+        <f>PRODUCT(D50,Valor_dolar)</f>
+        <v>4663.17</v>
+      </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C51" s="24" t="s">
@@ -2329,7 +2475,10 @@
       <c r="E51" s="30">
         <v>5</v>
       </c>
-      <c r="F51" s="26"/>
+      <c r="F51" s="26">
+        <f>PRODUCT(D51,Valor_dolar)</f>
+        <v>3431.97</v>
+      </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C52" s="24" t="s">
@@ -2341,7 +2490,10 @@
       <c r="E52" s="30">
         <v>14</v>
       </c>
-      <c r="F52" s="26"/>
+      <c r="F52" s="26">
+        <f>PRODUCT(D52,Valor_dolar)</f>
+        <v>3016.44</v>
+      </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C53" s="24" t="s">
@@ -2353,7 +2505,10 @@
       <c r="E53" s="30">
         <v>10</v>
       </c>
-      <c r="F53" s="26"/>
+      <c r="F53" s="26">
+        <f>PRODUCT(D53,Valor_dolar)</f>
+        <v>4011.66</v>
+      </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C54" s="24" t="s">
@@ -2365,7 +2520,10 @@
       <c r="E54" s="30">
         <v>4</v>
       </c>
-      <c r="F54" s="26"/>
+      <c r="F54" s="26">
+        <f>PRODUCT(D54,Valor_dolar)</f>
+        <v>2975.4</v>
+      </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C55" s="24" t="s">
@@ -2377,7 +2535,10 @@
       <c r="E55" s="30">
         <v>16</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="26">
+        <f>PRODUCT(D55,Valor_dolar)</f>
+        <v>4596.4799999999996</v>
+      </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C56" s="24" t="s">
@@ -2389,7 +2550,10 @@
       <c r="E56" s="30">
         <v>17</v>
       </c>
-      <c r="F56" s="26"/>
+      <c r="F56" s="26">
+        <f>PRODUCT(D56,Valor_dolar)</f>
+        <v>3903.93</v>
+      </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C57" s="24" t="s">
@@ -2401,7 +2565,10 @@
       <c r="E57" s="30">
         <v>8</v>
       </c>
-      <c r="F57" s="26"/>
+      <c r="F57" s="26">
+        <f>PRODUCT(D57,Valor_dolar)</f>
+        <v>4134.78</v>
+      </c>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C58" s="24" t="s">
@@ -2413,7 +2580,10 @@
       <c r="E58" s="30">
         <v>15</v>
       </c>
-      <c r="F58" s="26"/>
+      <c r="F58" s="26">
+        <f>PRODUCT(D58,Valor_dolar)</f>
+        <v>4227.12</v>
+      </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C59" s="24" t="s">
@@ -2425,7 +2595,10 @@
       <c r="E59" s="30">
         <v>10</v>
       </c>
-      <c r="F59" s="26"/>
+      <c r="F59" s="26">
+        <f>PRODUCT(D59,Valor_dolar)</f>
+        <v>3108.7799999999997</v>
+      </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C60" s="24" t="s">
@@ -2437,7 +2610,10 @@
       <c r="E60" s="30">
         <v>6</v>
       </c>
-      <c r="F60" s="26"/>
+      <c r="F60" s="26">
+        <f>PRODUCT(D60,Valor_dolar)</f>
+        <v>2883.06</v>
+      </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C61" s="24" t="s">
@@ -2449,7 +2625,10 @@
       <c r="E61" s="30">
         <v>19</v>
       </c>
-      <c r="F61" s="26"/>
+      <c r="F61" s="26">
+        <f>PRODUCT(D61,Valor_dolar)</f>
+        <v>3124.17</v>
+      </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C62" s="24" t="s">
@@ -2461,7 +2640,10 @@
       <c r="E62" s="30">
         <v>14</v>
       </c>
-      <c r="F62" s="26"/>
+      <c r="F62" s="26">
+        <f>PRODUCT(D62,Valor_dolar)</f>
+        <v>4837.59</v>
+      </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C63" s="24" t="s">
@@ -2473,7 +2655,10 @@
       <c r="E63" s="30">
         <v>16</v>
       </c>
-      <c r="F63" s="26"/>
+      <c r="F63" s="26">
+        <f>PRODUCT(D63,Valor_dolar)</f>
+        <v>4888.8900000000003</v>
+      </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C64" s="24" t="s">
@@ -2485,7 +2670,10 @@
       <c r="E64" s="30">
         <v>20</v>
       </c>
-      <c r="F64" s="26"/>
+      <c r="F64" s="26">
+        <f>PRODUCT(D64,Valor_dolar)</f>
+        <v>2698.38</v>
+      </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="24" t="s">
@@ -2497,7 +2685,10 @@
       <c r="E65" s="30">
         <v>18</v>
       </c>
-      <c r="F65" s="26"/>
+      <c r="F65" s="26">
+        <f>PRODUCT(D65,Valor_dolar)</f>
+        <v>2770.2</v>
+      </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" s="24" t="s">
@@ -2509,7 +2700,10 @@
       <c r="E66" s="30">
         <v>9</v>
       </c>
-      <c r="F66" s="26"/>
+      <c r="F66" s="26">
+        <f>PRODUCT(D66,Valor_dolar)</f>
+        <v>5006.88</v>
+      </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C67" s="24" t="s">
@@ -2521,7 +2715,10 @@
       <c r="E67" s="30">
         <v>8</v>
       </c>
-      <c r="F67" s="26"/>
+      <c r="F67" s="26">
+        <f>PRODUCT(D67,Valor_dolar)</f>
+        <v>3944.97</v>
+      </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C68" s="24" t="s">
@@ -2533,7 +2730,10 @@
       <c r="E68" s="30">
         <v>2</v>
       </c>
-      <c r="F68" s="26"/>
+      <c r="F68" s="26">
+        <f>PRODUCT(D68,Valor_dolar)</f>
+        <v>2570.13</v>
+      </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="24" t="s">
@@ -2545,7 +2745,10 @@
       <c r="E69" s="30">
         <v>17</v>
       </c>
-      <c r="F69" s="26"/>
+      <c r="F69" s="26">
+        <f>PRODUCT(D69,Valor_dolar)</f>
+        <v>4206.6000000000004</v>
+      </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" s="24" t="s">
@@ -2557,7 +2760,10 @@
       <c r="E70" s="30">
         <v>13</v>
       </c>
-      <c r="F70" s="26"/>
+      <c r="F70" s="26">
+        <f>PRODUCT(D70,Valor_dolar)</f>
+        <v>5109.4799999999996</v>
+      </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" s="24" t="s">
@@ -2569,7 +2775,10 @@
       <c r="E71" s="30">
         <v>8</v>
       </c>
-      <c r="F71" s="26"/>
+      <c r="F71" s="26">
+        <f>PRODUCT(D71,Valor_dolar)</f>
+        <v>2836.89</v>
+      </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C72" s="24" t="s">
@@ -2581,7 +2790,10 @@
       <c r="E72" s="30">
         <v>6</v>
       </c>
-      <c r="F72" s="26"/>
+      <c r="F72" s="26">
+        <f>PRODUCT(D72,Valor_dolar)</f>
+        <v>2985.66</v>
+      </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" s="24" t="s">
@@ -2593,7 +2805,10 @@
       <c r="E73" s="30">
         <v>19</v>
       </c>
-      <c r="F73" s="26"/>
+      <c r="F73" s="26">
+        <f>PRODUCT(D73,Valor_dolar)</f>
+        <v>3313.98</v>
+      </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" s="24" t="s">
@@ -2605,7 +2820,10 @@
       <c r="E74" s="30">
         <v>11</v>
       </c>
-      <c r="F74" s="26"/>
+      <c r="F74" s="26">
+        <f>PRODUCT(D74,Valor_dolar)</f>
+        <v>4868.37</v>
+      </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" s="24" t="s">
@@ -2617,7 +2835,10 @@
       <c r="E75" s="30">
         <v>14</v>
       </c>
-      <c r="F75" s="26"/>
+      <c r="F75" s="26">
+        <f>PRODUCT(D75,Valor_dolar)</f>
+        <v>2800.98</v>
+      </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" s="24" t="s">
@@ -2629,7 +2850,10 @@
       <c r="E76" s="30">
         <v>6</v>
       </c>
-      <c r="F76" s="26"/>
+      <c r="F76" s="26">
+        <f>PRODUCT(D76,Valor_dolar)</f>
+        <v>4257.8999999999996</v>
+      </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C77" s="24" t="s">
@@ -2641,7 +2865,10 @@
       <c r="E77" s="30">
         <v>19</v>
       </c>
-      <c r="F77" s="26"/>
+      <c r="F77" s="26">
+        <f>PRODUCT(D77,Valor_dolar)</f>
+        <v>2739.42</v>
+      </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C78" s="24" t="s">
@@ -2653,7 +2880,10 @@
       <c r="E78" s="30">
         <v>19</v>
       </c>
-      <c r="F78" s="26"/>
+      <c r="F78" s="26">
+        <f>PRODUCT(D78,Valor_dolar)</f>
+        <v>4442.58</v>
+      </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C79" s="24" t="s">
@@ -2665,7 +2895,10 @@
       <c r="E79" s="30">
         <v>1</v>
       </c>
-      <c r="F79" s="26"/>
+      <c r="F79" s="26">
+        <f>PRODUCT(D79,Valor_dolar)</f>
+        <v>4062.96</v>
+      </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C80" s="24" t="s">
@@ -2677,7 +2910,10 @@
       <c r="E80" s="30">
         <v>18</v>
       </c>
-      <c r="F80" s="26"/>
+      <c r="F80" s="26">
+        <f>PRODUCT(D80,Valor_dolar)</f>
+        <v>4411.8</v>
+      </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C81" s="24" t="s">
@@ -2689,7 +2925,10 @@
       <c r="E81" s="30">
         <v>1</v>
       </c>
-      <c r="F81" s="26"/>
+      <c r="F81" s="26">
+        <f>PRODUCT(D81,Valor_dolar)</f>
+        <v>3083.13</v>
+      </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C82" s="24" t="s">
@@ -2701,7 +2940,10 @@
       <c r="E82" s="30">
         <v>18</v>
       </c>
-      <c r="F82" s="26"/>
+      <c r="F82" s="26">
+        <f>PRODUCT(D82,Valor_dolar)</f>
+        <v>3832.11</v>
+      </c>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C83" s="24" t="s">
@@ -2713,7 +2955,10 @@
       <c r="E83" s="30">
         <v>2</v>
       </c>
-      <c r="F83" s="26"/>
+      <c r="F83" s="26">
+        <f>PRODUCT(D83,Valor_dolar)</f>
+        <v>4021.92</v>
+      </c>
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C84" s="24" t="s">
@@ -2725,7 +2970,10 @@
       <c r="E84" s="30">
         <v>3</v>
       </c>
-      <c r="F84" s="26"/>
+      <c r="F84" s="26">
+        <f>PRODUCT(D84,Valor_dolar)</f>
+        <v>4858.1099999999997</v>
+      </c>
     </row>
     <row r="85" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C85" s="24" t="s">
@@ -2737,7 +2985,10 @@
       <c r="E85" s="30">
         <v>5</v>
       </c>
-      <c r="F85" s="26"/>
+      <c r="F85" s="26">
+        <f>PRODUCT(D85,Valor_dolar)</f>
+        <v>5078.7</v>
+      </c>
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C86" s="24" t="s">
@@ -2749,7 +3000,10 @@
       <c r="E86" s="30">
         <v>10</v>
       </c>
-      <c r="F86" s="26"/>
+      <c r="F86" s="26">
+        <f>PRODUCT(D86,Valor_dolar)</f>
+        <v>4186.08</v>
+      </c>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C87" s="24" t="s">
@@ -2761,7 +3015,10 @@
       <c r="E87" s="30">
         <v>10</v>
       </c>
-      <c r="F87" s="26"/>
+      <c r="F87" s="26">
+        <f>PRODUCT(D87,Valor_dolar)</f>
+        <v>4473.3599999999997</v>
+      </c>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E88" s="29"/>

</xml_diff>